<commit_message>
Curry's new model outputs after refitting Sunday Oct 20, 2019
</commit_message>
<xml_diff>
--- a/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
+++ b/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
@@ -1315,36 +1315,36 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>4026916.85943786</v>
+        <v>4405706.64402051</v>
       </c>
       <c r="B57" t="n">
-        <v>1552499.77578859</v>
+        <v>1587508.02938422</v>
       </c>
       <c r="C57" t="n">
-        <v>1810115.94515566</v>
+        <v>2203513.10981581</v>
       </c>
       <c r="D57" t="n">
-        <v>1038120.82780834</v>
+        <v>1560756.44183447</v>
       </c>
       <c r="E57" t="n">
-        <v>1164082.96370863</v>
+        <v>1217252.51734373</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2330461.29826415</v>
+        <v>2364640.68026053</v>
       </c>
       <c r="B58" t="n">
-        <v>818675.370794947</v>
+        <v>821493.35079737</v>
       </c>
       <c r="C58" t="n">
-        <v>2873472.86911456</v>
+        <v>2905600.53879869</v>
       </c>
       <c r="D58" t="n">
-        <v>2467763.73849173</v>
+        <v>2375950.28114173</v>
       </c>
       <c r="E58" t="n">
-        <v>1538607.30999964</v>
+        <v>1543355.63842831</v>
       </c>
     </row>
   </sheetData>
@@ -1380,971 +1380,971 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>280492.572394666</v>
+        <v>276578.552373643</v>
       </c>
       <c r="B2" t="n">
-        <v>177271.784303371</v>
+        <v>174834.281025996</v>
       </c>
       <c r="C2" t="n">
-        <v>902452.55787324</v>
+        <v>891173.008331618</v>
       </c>
       <c r="D2" t="n">
-        <v>1006924.8046063</v>
+        <v>994257.773170301</v>
       </c>
       <c r="E2" t="n">
-        <v>295748.382115025</v>
+        <v>291395.323257675</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1227987.92057834</v>
+        <v>1224565.06065252</v>
       </c>
       <c r="B3" t="n">
-        <v>511874.538892071</v>
+        <v>510683.050314863</v>
       </c>
       <c r="C3" t="n">
-        <v>596840.165455162</v>
+        <v>593791.176975579</v>
       </c>
       <c r="D3" t="n">
-        <v>1166183.23856445</v>
+        <v>1163025.39794358</v>
       </c>
       <c r="E3" t="n">
-        <v>835095.577425403</v>
+        <v>833048.316096084</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>24336348.0652932</v>
+        <v>24301378.9195327</v>
       </c>
       <c r="B4" t="n">
-        <v>223126.741324511</v>
+        <v>222840.608249556</v>
       </c>
       <c r="C4" t="n">
-        <v>505148.256972446</v>
+        <v>504269.3644836</v>
       </c>
       <c r="D4" t="n">
-        <v>3730082.49021648</v>
+        <v>3726341.66980578</v>
       </c>
       <c r="E4" t="n">
-        <v>1889703.49134918</v>
+        <v>1887642.35087249</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5178802.61850462</v>
+        <v>5160347.98288509</v>
       </c>
       <c r="B5" t="n">
-        <v>220544.151784834</v>
+        <v>219741.159003453</v>
       </c>
       <c r="C5" t="n">
-        <v>1874195.0786093</v>
+        <v>1868341.49514396</v>
       </c>
       <c r="D5" t="n">
-        <v>2105554.37255064</v>
+        <v>2099605.0502669</v>
       </c>
       <c r="E5" t="n">
-        <v>672091.708879028</v>
+        <v>669303.277233215</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2337134.31023397</v>
+        <v>2329214.52733204</v>
       </c>
       <c r="B6" t="n">
-        <v>142157.53935245</v>
+        <v>141679.585523878</v>
       </c>
       <c r="C6" t="n">
-        <v>801558.487323993</v>
+        <v>799410.91354077</v>
       </c>
       <c r="D6" t="n">
-        <v>1090619.22241948</v>
+        <v>1088198.79502</v>
       </c>
       <c r="E6" t="n">
-        <v>201879.412896023</v>
+        <v>201262.796181305</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1426763.75779244</v>
+        <v>1418524.09594491</v>
       </c>
       <c r="B7" t="n">
-        <v>120841.636908133</v>
+        <v>120161.557353414</v>
       </c>
       <c r="C7" t="n">
-        <v>802893.620924332</v>
+        <v>798861.254148178</v>
       </c>
       <c r="D7" t="n">
-        <v>675517.959207873</v>
+        <v>673322.91406883</v>
       </c>
       <c r="E7" t="n">
-        <v>78785.8094476358</v>
+        <v>78460.418996627</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5684294.46957606</v>
+        <v>5660544.96695114</v>
       </c>
       <c r="B8" t="n">
-        <v>142372.629462142</v>
+        <v>141798.955126113</v>
       </c>
       <c r="C8" t="n">
-        <v>1314578.75317348</v>
+        <v>1309899.31919325</v>
       </c>
       <c r="D8" t="n">
-        <v>1004889.87653983</v>
+        <v>1001161.50096243</v>
       </c>
       <c r="E8" t="n">
-        <v>142049.087243396</v>
+        <v>141514.301621546</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>20942827.0250883</v>
+        <v>20904378.7196866</v>
       </c>
       <c r="B9" t="n">
-        <v>324268.365645301</v>
+        <v>323719.511424367</v>
       </c>
       <c r="C9" t="n">
-        <v>1959960.71856296</v>
+        <v>1957017.094043</v>
       </c>
       <c r="D9" t="n">
-        <v>1027774.6460737</v>
+        <v>1025634.9127658</v>
       </c>
       <c r="E9" t="n">
-        <v>319058.320140243</v>
+        <v>317910.461131596</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>4616267.28596478</v>
+        <v>4590714.78320268</v>
       </c>
       <c r="B10" t="n">
-        <v>351947.518354763</v>
+        <v>349991.524475971</v>
       </c>
       <c r="C10" t="n">
-        <v>2735547.03564426</v>
+        <v>2722279.57269316</v>
       </c>
       <c r="D10" t="n">
-        <v>1369382.72658139</v>
+        <v>1362086.30104241</v>
       </c>
       <c r="E10" t="n">
-        <v>1251270.445943</v>
+        <v>1244844.3922326</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1135359.42092187</v>
+        <v>1122324.57869894</v>
       </c>
       <c r="B11" t="n">
-        <v>153233.598285812</v>
+        <v>151401.307168642</v>
       </c>
       <c r="C11" t="n">
-        <v>890849.386176816</v>
+        <v>881866.336869179</v>
       </c>
       <c r="D11" t="n">
-        <v>1238925.18490036</v>
+        <v>1228132.94740325</v>
       </c>
       <c r="E11" t="n">
-        <v>53133.7168691681</v>
+        <v>52320.1835689389</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>193686.07679745</v>
+        <v>183932.629384088</v>
       </c>
       <c r="B12" t="n">
-        <v>29791.225977809</v>
+        <v>28272.9693721716</v>
       </c>
       <c r="C12" t="n">
-        <v>343990.286509483</v>
+        <v>327582.617293339</v>
       </c>
       <c r="D12" t="n">
-        <v>477569.194953669</v>
+        <v>458699.574507072</v>
       </c>
       <c r="E12" t="n">
-        <v>25939.2782007587</v>
+        <v>24423.4137182811</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>632049.172892099</v>
+        <v>627509.087761444</v>
       </c>
       <c r="B13" t="n">
-        <v>32958.1237914212</v>
+        <v>32731.730430268</v>
       </c>
       <c r="C13" t="n">
-        <v>234948.14708946</v>
+        <v>233585.477125937</v>
       </c>
       <c r="D13" t="n">
-        <v>229984.344061718</v>
+        <v>228607.231811913</v>
       </c>
       <c r="E13" t="n">
-        <v>4958.5083532886</v>
+        <v>4897.57543673656</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3093799.8326632</v>
+        <v>3079180.7068905</v>
       </c>
       <c r="B14" t="n">
-        <v>12281.7805107632</v>
+        <v>12176.7015881875</v>
       </c>
       <c r="C14" t="n">
-        <v>1187453.32628497</v>
+        <v>1184463.76219245</v>
       </c>
       <c r="D14" t="n">
-        <v>1066958.1653041</v>
+        <v>1064830.98438434</v>
       </c>
       <c r="E14" t="n">
-        <v>96718.5442762316</v>
+        <v>96228.6941403656</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1594204.64559325</v>
+        <v>1580050.45768817</v>
       </c>
       <c r="B15" t="n">
-        <v>76291.924099966</v>
+        <v>75627.6706805097</v>
       </c>
       <c r="C15" t="n">
-        <v>1893938.79845609</v>
+        <v>1879850.08525333</v>
       </c>
       <c r="D15" t="n">
-        <v>1202953.45480843</v>
+        <v>1195735.44781466</v>
       </c>
       <c r="E15" t="n">
-        <v>265010.271855951</v>
+        <v>262392.61882948</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>340012.465670716</v>
+        <v>334328.252487236</v>
       </c>
       <c r="B16" t="n">
-        <v>126804.593353828</v>
+        <v>126004.834210881</v>
       </c>
       <c r="C16" t="n">
-        <v>1836868.93890419</v>
+        <v>1826964.42190545</v>
       </c>
       <c r="D16" t="n">
-        <v>2315891.53961091</v>
+        <v>2305653.00952958</v>
       </c>
       <c r="E16" t="n">
-        <v>229641.911855838</v>
+        <v>228177.412478799</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3782290.84852626</v>
+        <v>3769806.21689585</v>
       </c>
       <c r="B17" t="n">
-        <v>527530.921488494</v>
+        <v>525732.154587301</v>
       </c>
       <c r="C17" t="n">
-        <v>1447071.38094098</v>
+        <v>1443431.79938304</v>
       </c>
       <c r="D17" t="n">
-        <v>1186092.93916222</v>
+        <v>1182594.47356981</v>
       </c>
       <c r="E17" t="n">
-        <v>14843.8366910513</v>
+        <v>14680.0150350691</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>13718681.1066707</v>
+        <v>13708608.4613785</v>
       </c>
       <c r="B18" t="n">
-        <v>870633.764362023</v>
+        <v>869976.938831844</v>
       </c>
       <c r="C18" t="n">
-        <v>1902384.98261733</v>
+        <v>1901243.63317692</v>
       </c>
       <c r="D18" t="n">
-        <v>1548873.90560852</v>
+        <v>1547811.17049409</v>
       </c>
       <c r="E18" t="n">
-        <v>580729.236051706</v>
+        <v>579827.621013041</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>15463979.2963114</v>
+        <v>15426412.0582306</v>
       </c>
       <c r="B19" t="n">
-        <v>96865.2904421437</v>
+        <v>96015.8623337595</v>
       </c>
       <c r="C19" t="n">
-        <v>2440395.5346124</v>
+        <v>2435352.2984598</v>
       </c>
       <c r="D19" t="n">
-        <v>2392284.37263067</v>
+        <v>2388859.40641703</v>
       </c>
       <c r="E19" t="n">
-        <v>1311921.02259516</v>
+        <v>1307289.23932738</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>5159221.68530891</v>
+        <v>5146995.48720011</v>
       </c>
       <c r="B20" t="n">
-        <v>458782.237985286</v>
+        <v>457599.197580798</v>
       </c>
       <c r="C20" t="n">
-        <v>6976133.95507893</v>
+        <v>6960611.23717385</v>
       </c>
       <c r="D20" t="n">
-        <v>3955342.45965401</v>
+        <v>3947105.16286262</v>
       </c>
       <c r="E20" t="n">
-        <v>2757761.84175488</v>
+        <v>2750538.47693667</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1688135.42404288</v>
+        <v>1677035.1393432</v>
       </c>
       <c r="B21" t="n">
-        <v>740673.303852158</v>
+        <v>735360.81982849</v>
       </c>
       <c r="C21" t="n">
-        <v>3523655.93664317</v>
+        <v>3505253.78666771</v>
       </c>
       <c r="D21" t="n">
-        <v>2765349.7569389</v>
+        <v>2750401.67598035</v>
       </c>
       <c r="E21" t="n">
-        <v>1507694.71422842</v>
+        <v>1497098.72556133</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>17943220.3880591</v>
+        <v>17926889.5597048</v>
       </c>
       <c r="B22" t="n">
-        <v>2421238.39794382</v>
+        <v>2419214.17766675</v>
       </c>
       <c r="C22" t="n">
-        <v>2422483.45953312</v>
+        <v>2419970.24856515</v>
       </c>
       <c r="D22" t="n">
-        <v>7660443.14412031</v>
+        <v>7654025.46041335</v>
       </c>
       <c r="E22" t="n">
-        <v>3150234.84218656</v>
+        <v>3147084.41719607</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>13447311.4804582</v>
+        <v>13440247.9595964</v>
       </c>
       <c r="B23" t="n">
-        <v>644405.79196586</v>
+        <v>644055.943107989</v>
       </c>
       <c r="C23" t="n">
-        <v>2635008.60552283</v>
+        <v>2633879.26521037</v>
       </c>
       <c r="D23" t="n">
-        <v>4294677.66327681</v>
+        <v>4293080.15933608</v>
       </c>
       <c r="E23" t="n">
-        <v>2897893.62730967</v>
+        <v>2896673.72240236</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>6887734.0796818</v>
+        <v>6882451.28823552</v>
       </c>
       <c r="B24" t="n">
-        <v>542914.620779718</v>
+        <v>542603.608813087</v>
       </c>
       <c r="C24" t="n">
-        <v>2388959.82477268</v>
+        <v>2387371.7452243</v>
       </c>
       <c r="D24" t="n">
-        <v>7239609.33584629</v>
+        <v>7236474.15512163</v>
       </c>
       <c r="E24" t="n">
-        <v>6937376.94214315</v>
+        <v>6934391.19886809</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>834069.607884201</v>
+        <v>833126.611266666</v>
       </c>
       <c r="B25" t="n">
-        <v>434468.198463539</v>
+        <v>433979.708283939</v>
       </c>
       <c r="C25" t="n">
-        <v>2015591.25913479</v>
+        <v>2013670.64836189</v>
       </c>
       <c r="D25" t="n">
-        <v>4356941.1437001</v>
+        <v>4354320.13233604</v>
       </c>
       <c r="E25" t="n">
-        <v>5714903.79325193</v>
+        <v>5711691.69675829</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>4258967.37320722</v>
+        <v>4252233.25526641</v>
       </c>
       <c r="B26" t="n">
-        <v>387990.61344493</v>
+        <v>387501.818984514</v>
       </c>
       <c r="C26" t="n">
-        <v>1258739.7867712</v>
+        <v>1257204.07694389</v>
       </c>
       <c r="D26" t="n">
-        <v>5115989.27695546</v>
+        <v>5111676.44371179</v>
       </c>
       <c r="E26" t="n">
-        <v>2225081.00049386</v>
+        <v>2223118.70745475</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2803855.66310455</v>
+        <v>2794832.61270317</v>
       </c>
       <c r="B27" t="n">
-        <v>355902.080043595</v>
+        <v>354828.098574204</v>
       </c>
       <c r="C27" t="n">
-        <v>927669.5955879</v>
+        <v>925110.634473635</v>
       </c>
       <c r="D27" t="n">
-        <v>6515702.49416988</v>
+        <v>6504819.37796044</v>
       </c>
       <c r="E27" t="n">
-        <v>1503621.31778358</v>
+        <v>1500731.21170249</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>12169655.088784</v>
+        <v>12166907.99944</v>
       </c>
       <c r="B28" t="n">
-        <v>877798.789588314</v>
+        <v>877631.766427054</v>
       </c>
       <c r="C28" t="n">
-        <v>2508334.34303789</v>
+        <v>2507847.29519868</v>
       </c>
       <c r="D28" t="n">
-        <v>8197250.23811127</v>
+        <v>8195893.99315057</v>
       </c>
       <c r="E28" t="n">
-        <v>3650795.17205646</v>
+        <v>3650053.07174421</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>11226219.6560904</v>
+        <v>11222968.9615815</v>
       </c>
       <c r="B29" t="n">
-        <v>1161345.26454786</v>
+        <v>1161087.18648867</v>
       </c>
       <c r="C29" t="n">
-        <v>6209267.45784261</v>
+        <v>6207753.6004993</v>
       </c>
       <c r="D29" t="n">
-        <v>10416192.2090193</v>
+        <v>10413845.2261317</v>
       </c>
       <c r="E29" t="n">
-        <v>1963644.25587232</v>
+        <v>1963139.43814492</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>4396050.95944555</v>
+        <v>4390338.79339924</v>
       </c>
       <c r="B30" t="n">
-        <v>977897.662456532</v>
+        <v>976802.97065121</v>
       </c>
       <c r="C30" t="n">
-        <v>6182599.26286106</v>
+        <v>6175916.63225796</v>
       </c>
       <c r="D30" t="n">
-        <v>6454919.78167244</v>
+        <v>6448545.32825452</v>
       </c>
       <c r="E30" t="n">
-        <v>3481130.6531801</v>
+        <v>3477020.39581145</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>5912516.6863788</v>
+        <v>5902775.80856216</v>
       </c>
       <c r="B31" t="n">
-        <v>885044.316387286</v>
+        <v>883698.88582968</v>
       </c>
       <c r="C31" t="n">
-        <v>3621211.36802422</v>
+        <v>3616256.78407975</v>
       </c>
       <c r="D31" t="n">
-        <v>15962382.0007476</v>
+        <v>15945360.6677112</v>
       </c>
       <c r="E31" t="n">
-        <v>4152329.73446594</v>
+        <v>4146311.57202565</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>4045070.88555976</v>
+        <v>4039704.92993661</v>
       </c>
       <c r="B32" t="n">
-        <v>1566023.27980209</v>
+        <v>1564398.71468256</v>
       </c>
       <c r="C32" t="n">
-        <v>4045329.19237137</v>
+        <v>4041526.76273218</v>
       </c>
       <c r="D32" t="n">
-        <v>22750393.3330111</v>
+        <v>22733547.8663982</v>
       </c>
       <c r="E32" t="n">
-        <v>4807562.78632773</v>
+        <v>4803243.59102978</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>13242285.3512991</v>
+        <v>13236400.7809929</v>
       </c>
       <c r="B33" t="n">
-        <v>1444064.23070069</v>
+        <v>1443559.19966165</v>
       </c>
       <c r="C33" t="n">
-        <v>2710960.10599351</v>
+        <v>2709998.24104081</v>
       </c>
       <c r="D33" t="n">
-        <v>10843878.8936465</v>
+        <v>10840335.4816904</v>
       </c>
       <c r="E33" t="n">
-        <v>4476444.63722483</v>
+        <v>4474903.24479452</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>18399540.3590962</v>
+        <v>18387943.0947472</v>
       </c>
       <c r="B34" t="n">
-        <v>1649522.55212512</v>
+        <v>1648709.74092832</v>
       </c>
       <c r="C34" t="n">
-        <v>2330344.2866557</v>
+        <v>2329001.64409408</v>
       </c>
       <c r="D34" t="n">
-        <v>14114687.1255001</v>
+        <v>14108237.5361751</v>
       </c>
       <c r="E34" t="n">
-        <v>4594328.42000555</v>
+        <v>4591849.99815862</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>3025846.07262494</v>
+        <v>3024092.18718042</v>
       </c>
       <c r="B35" t="n">
-        <v>1602294.22877101</v>
+        <v>1601329.23479073</v>
       </c>
       <c r="C35" t="n">
-        <v>3586267.90859137</v>
+        <v>3584362.92726945</v>
       </c>
       <c r="D35" t="n">
-        <v>11344834.697877</v>
+        <v>11339737.4079661</v>
       </c>
       <c r="E35" t="n">
-        <v>4680687.22395326</v>
+        <v>4678485.6804553</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>890763.222686602</v>
+        <v>888485.583524104</v>
       </c>
       <c r="B36" t="n">
-        <v>258915.048964573</v>
+        <v>258142.997824125</v>
       </c>
       <c r="C36" t="n">
-        <v>886811.148977108</v>
+        <v>885146.195871819</v>
       </c>
       <c r="D36" t="n">
-        <v>6835765.05003025</v>
+        <v>6828118.5109713</v>
       </c>
       <c r="E36" t="n">
-        <v>1854523.36224487</v>
+        <v>1852110.34808976</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1518562.35304501</v>
+        <v>1514946.55028179</v>
       </c>
       <c r="B37" t="n">
-        <v>543617.890477848</v>
+        <v>542481.303224469</v>
       </c>
       <c r="C37" t="n">
-        <v>1165243.48423282</v>
+        <v>1162944.31804395</v>
       </c>
       <c r="D37" t="n">
-        <v>3583277.97363538</v>
+        <v>3578659.35042967</v>
       </c>
       <c r="E37" t="n">
-        <v>969281.523336312</v>
+        <v>967421.618015631</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>7012520.1765226</v>
+        <v>7006237.60747499</v>
       </c>
       <c r="B38" t="n">
-        <v>1848176.39837222</v>
+        <v>1846756.65028382</v>
       </c>
       <c r="C38" t="n">
-        <v>3078307.75851465</v>
+        <v>3076119.59075156</v>
       </c>
       <c r="D38" t="n">
-        <v>4755854.04431993</v>
+        <v>4752677.18836178</v>
       </c>
       <c r="E38" t="n">
-        <v>3564404.07907662</v>
+        <v>3561838.80723473</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1748677.04615078</v>
+        <v>1742174.42169216</v>
       </c>
       <c r="B39" t="n">
-        <v>1042391.05792073</v>
+        <v>1038351.18179196</v>
       </c>
       <c r="C39" t="n">
-        <v>2597688.72282005</v>
+        <v>2591907.19753614</v>
       </c>
       <c r="D39" t="n">
-        <v>7152200.16583971</v>
+        <v>7136560.91107415</v>
       </c>
       <c r="E39" t="n">
-        <v>1666069.96913165</v>
+        <v>1661678.25595062</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>845676.127308125</v>
+        <v>844876.707891008</v>
       </c>
       <c r="B40" t="n">
-        <v>506550.27971841</v>
+        <v>506062.55495399</v>
       </c>
       <c r="C40" t="n">
-        <v>4162350.06027438</v>
+        <v>4160824.94023345</v>
       </c>
       <c r="D40" t="n">
-        <v>2599197.47587467</v>
+        <v>2597572.17863223</v>
       </c>
       <c r="E40" t="n">
-        <v>601871.855342475</v>
+        <v>601206.962430473</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>194768.997962748</v>
+        <v>193989.611029551</v>
       </c>
       <c r="B41" t="n">
-        <v>175174.692095889</v>
+        <v>174338.532840884</v>
       </c>
       <c r="C41" t="n">
-        <v>1551144.38722094</v>
+        <v>1549679.6569901</v>
       </c>
       <c r="D41" t="n">
-        <v>4513439.26495282</v>
+        <v>4508229.67348237</v>
       </c>
       <c r="E41" t="n">
-        <v>1595815.69036007</v>
+        <v>1593464.61207731</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>316361.369659673</v>
+        <v>314970.823885078</v>
       </c>
       <c r="B42" t="n">
-        <v>484633.047167341</v>
+        <v>481639.645227682</v>
       </c>
       <c r="C42" t="n">
-        <v>3032027.71247548</v>
+        <v>3030405.06984201</v>
       </c>
       <c r="D42" t="n">
-        <v>2067729.60672988</v>
+        <v>2065235.09925069</v>
       </c>
       <c r="E42" t="n">
-        <v>1751966.32626989</v>
+        <v>1750037.5830476</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2593940.7468526</v>
+        <v>2591074.16575682</v>
       </c>
       <c r="B43" t="n">
-        <v>2131962.52039654</v>
+        <v>2129291.78554283</v>
       </c>
       <c r="C43" t="n">
-        <v>2128137.80776055</v>
+        <v>2127008.05990141</v>
       </c>
       <c r="D43" t="n">
-        <v>10356675.6589852</v>
+        <v>10352421.1683057</v>
       </c>
       <c r="E43" t="n">
-        <v>3389222.57981263</v>
+        <v>3387686.67258656</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>548567.939848724</v>
+        <v>547346.888283056</v>
       </c>
       <c r="B44" t="n">
-        <v>1007979.4698569</v>
+        <v>1005725.57939027</v>
       </c>
       <c r="C44" t="n">
-        <v>6022954.41050183</v>
+        <v>6020749.00231191</v>
       </c>
       <c r="D44" t="n">
-        <v>7784895.26160578</v>
+        <v>7780470.39316064</v>
       </c>
       <c r="E44" t="n">
-        <v>2291851.44110008</v>
+        <v>2290389.95047015</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2649994.42406843</v>
+        <v>2647163.79616081</v>
       </c>
       <c r="B45" t="n">
-        <v>1570529.45515275</v>
+        <v>1568912.91757652</v>
       </c>
       <c r="C45" t="n">
-        <v>3390639.98050381</v>
+        <v>3389013.08484526</v>
       </c>
       <c r="D45" t="n">
-        <v>7153099.55997441</v>
+        <v>7148683.93725043</v>
       </c>
       <c r="E45" t="n">
-        <v>2777961.87671016</v>
+        <v>2776018.12753687</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3112513.13608123</v>
+        <v>3107283.96412581</v>
       </c>
       <c r="B46" t="n">
-        <v>2309114.62554841</v>
+        <v>2304818.68305184</v>
       </c>
       <c r="C46" t="n">
-        <v>5498574.09067079</v>
+        <v>5493187.67746471</v>
       </c>
       <c r="D46" t="n">
-        <v>5969910.79733928</v>
+        <v>5962532.41636901</v>
       </c>
       <c r="E46" t="n">
-        <v>4807891.31645388</v>
+        <v>4800517.24582615</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>3277801.38091523</v>
+        <v>3272707.5986842</v>
       </c>
       <c r="B47" t="n">
-        <v>2528131.53333538</v>
+        <v>2524158.31143013</v>
       </c>
       <c r="C47" t="n">
-        <v>6662593.59261084</v>
+        <v>6654497.81083594</v>
       </c>
       <c r="D47" t="n">
-        <v>6572692.39525076</v>
+        <v>6565684.25146314</v>
       </c>
       <c r="E47" t="n">
-        <v>2336190.44122499</v>
+        <v>2333562.71027486</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>4699580.45892978</v>
+        <v>4695644.09449449</v>
       </c>
       <c r="B48" t="n">
-        <v>1399765.74146378</v>
+        <v>1398341.92902897</v>
       </c>
       <c r="C48" t="n">
-        <v>3746491.28492215</v>
+        <v>3743453.86183774</v>
       </c>
       <c r="D48" t="n">
-        <v>11131031.7711472</v>
+        <v>11123394.9490563</v>
       </c>
       <c r="E48" t="n">
-        <v>2489316.20717834</v>
+        <v>2486916.22278973</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>6576090.10862043</v>
+        <v>6571919.06682822</v>
       </c>
       <c r="B49" t="n">
-        <v>1628896.73990133</v>
+        <v>1627824.25707974</v>
       </c>
       <c r="C49" t="n">
-        <v>3975120.99713332</v>
+        <v>3972969.89955667</v>
       </c>
       <c r="D49" t="n">
-        <v>4220704.72933101</v>
+        <v>4218596.23575175</v>
       </c>
       <c r="E49" t="n">
-        <v>4159898.06872693</v>
+        <v>4157857.50019974</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>4972634.66364683</v>
+        <v>4964012.43802971</v>
       </c>
       <c r="B50" t="n">
-        <v>1368182.53795979</v>
+        <v>1365507.67123603</v>
       </c>
       <c r="C50" t="n">
-        <v>4349839.81338041</v>
+        <v>4343039.23096607</v>
       </c>
       <c r="D50" t="n">
-        <v>3648784.46110574</v>
+        <v>3642985.01722473</v>
       </c>
       <c r="E50" t="n">
-        <v>3178842.05431944</v>
+        <v>3173534.32785121</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>8116758.42465348</v>
+        <v>8099474.58931948</v>
       </c>
       <c r="B51" t="n">
-        <v>1367816.97796947</v>
+        <v>1364780.14818682</v>
       </c>
       <c r="C51" t="n">
-        <v>2425886.39376461</v>
+        <v>2421224.1436332</v>
       </c>
       <c r="D51" t="n">
-        <v>4697850.74534815</v>
+        <v>4689146.40433662</v>
       </c>
       <c r="E51" t="n">
-        <v>2230093.46186686</v>
+        <v>2225800.01970357</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>4245486.70675063</v>
+        <v>4235719.12242102</v>
       </c>
       <c r="B52" t="n">
-        <v>836766.588878826</v>
+        <v>833816.927896934</v>
       </c>
       <c r="C52" t="n">
-        <v>2140755.53902472</v>
+        <v>2135968.06887827</v>
       </c>
       <c r="D52" t="n">
-        <v>4019030.24609019</v>
+        <v>4010835.51229691</v>
       </c>
       <c r="E52" t="n">
-        <v>1739779.97566238</v>
+        <v>1735590.23183467</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>13145613.1423046</v>
+        <v>13141528.1867971</v>
       </c>
       <c r="B53" t="n">
-        <v>1420113.92669054</v>
+        <v>1419774.25104763</v>
       </c>
       <c r="C53" t="n">
-        <v>3847105.51477763</v>
+        <v>3845872.43272374</v>
       </c>
       <c r="D53" t="n">
-        <v>3697256.69280626</v>
+        <v>3696037.21468247</v>
       </c>
       <c r="E53" t="n">
-        <v>514136.109755338</v>
+        <v>513858.58068414</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>15767822.6439574</v>
+        <v>15763315.3012893</v>
       </c>
       <c r="B54" t="n">
-        <v>2475475.37290304</v>
+        <v>2473876.01750705</v>
       </c>
       <c r="C54" t="n">
-        <v>4170967.89563265</v>
+        <v>4169784.02921601</v>
       </c>
       <c r="D54" t="n">
-        <v>6348922.5346832</v>
+        <v>6347212.37502937</v>
       </c>
       <c r="E54" t="n">
-        <v>2685274.15618863</v>
+        <v>2684432.27201083</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>9739300.96163161</v>
+        <v>9733410.46183534</v>
       </c>
       <c r="B55" t="n">
-        <v>3164582.17144042</v>
+        <v>3162505.47782539</v>
       </c>
       <c r="C55" t="n">
-        <v>3347382.61352491</v>
+        <v>3345232.32432452</v>
       </c>
       <c r="D55" t="n">
-        <v>8058938.18815386</v>
+        <v>8054589.56249761</v>
       </c>
       <c r="E55" t="n">
-        <v>5560687.00070683</v>
+        <v>5557547.67974066</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>4090012.68153057</v>
+        <v>4086925.62991241</v>
       </c>
       <c r="B56" t="n">
-        <v>2390419.4143596</v>
+        <v>2388491.48625303</v>
       </c>
       <c r="C56" t="n">
-        <v>4078349.35518737</v>
+        <v>4075693.58064813</v>
       </c>
       <c r="D56" t="n">
-        <v>9845868.57872976</v>
+        <v>9840113.3322558</v>
       </c>
       <c r="E56" t="n">
-        <v>5489366.24392365</v>
+        <v>5486291.54145378</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2833657.01040271</v>
+        <v>3067970.1707458</v>
       </c>
       <c r="B57" t="n">
-        <v>1411002.51577714</v>
+        <v>1292122.83030637</v>
       </c>
       <c r="C57" t="n">
-        <v>4617849.18967567</v>
+        <v>4704907.93181197</v>
       </c>
       <c r="D57" t="n">
-        <v>4951848.10690051</v>
+        <v>4495954.05218515</v>
       </c>
       <c r="E57" t="n">
-        <v>3345891.3479101</v>
+        <v>3602429.93779496</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>5523590.33885266</v>
+        <v>5543863.9901118</v>
       </c>
       <c r="B58" t="n">
-        <v>1026275.69555222</v>
+        <v>1029963.20319573</v>
       </c>
       <c r="C58" t="n">
-        <v>5892190.57987315</v>
+        <v>5896769.41891236</v>
       </c>
       <c r="D58" t="n">
-        <v>13164062.5274062</v>
+        <v>13091748.9829389</v>
       </c>
       <c r="E58" t="n">
-        <v>2023819.30924335</v>
+        <v>2056749.6512372</v>
       </c>
     </row>
   </sheetData>
@@ -2380,971 +2380,971 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>619252.572329667</v>
+        <v>615338.552308645</v>
       </c>
       <c r="B2" t="n">
-        <v>380575.784250372</v>
+        <v>378138.280972998</v>
       </c>
       <c r="C2" t="n">
-        <v>1807810.55785729</v>
+        <v>1796531.00831567</v>
       </c>
       <c r="D2" t="n">
-        <v>2004526.8045393</v>
+        <v>1991859.7731033</v>
       </c>
       <c r="E2" t="n">
-        <v>684002.382144826</v>
+        <v>679649.323287476</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2185107.92060284</v>
+        <v>2181685.06067702</v>
       </c>
       <c r="B3" t="n">
-        <v>760574.5389503</v>
+        <v>759383.050373091</v>
       </c>
       <c r="C3" t="n">
-        <v>1946444.16537317</v>
+        <v>1943395.17689359</v>
       </c>
       <c r="D3" t="n">
-        <v>2015759.23860769</v>
+        <v>2012601.39798683</v>
       </c>
       <c r="E3" t="n">
-        <v>1307865.57746675</v>
+        <v>1305818.31613743</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>48662274.0630942</v>
+        <v>48627304.9173338</v>
       </c>
       <c r="B4" t="n">
-        <v>398146.741377621</v>
+        <v>397860.608302665</v>
       </c>
       <c r="C4" t="n">
-        <v>1222946.25707876</v>
+        <v>1222067.36458991</v>
       </c>
       <c r="D4" t="n">
-        <v>5174690.48987449</v>
+        <v>5170949.66946379</v>
       </c>
       <c r="E4" t="n">
-        <v>2886315.49133238</v>
+        <v>2884254.3508557</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8933987.61838363</v>
+        <v>8915532.9827641</v>
       </c>
       <c r="B5" t="n">
-        <v>394880.151734837</v>
+        <v>394077.158953457</v>
       </c>
       <c r="C5" t="n">
-        <v>2890640.07853631</v>
+        <v>2884786.49507096</v>
       </c>
       <c r="D5" t="n">
-        <v>2909800.37245924</v>
+        <v>2903851.0501755</v>
       </c>
       <c r="E5" t="n">
-        <v>1376527.70893693</v>
+        <v>1373739.27729112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5553342.31047937</v>
+        <v>5545422.52757744</v>
       </c>
       <c r="B6" t="n">
-        <v>344783.539305652</v>
+        <v>344305.58547708</v>
       </c>
       <c r="C6" t="n">
-        <v>1557198.4873481</v>
+        <v>1555050.91356487</v>
       </c>
       <c r="D6" t="n">
-        <v>1727483.22240808</v>
+        <v>1725062.7950086</v>
       </c>
       <c r="E6" t="n">
-        <v>440709.412939345</v>
+        <v>440092.796224627</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3984203.75800845</v>
+        <v>3975964.09616092</v>
       </c>
       <c r="B7" t="n">
-        <v>314713.636913835</v>
+        <v>314033.557359116</v>
       </c>
       <c r="C7" t="n">
-        <v>1826115.62105534</v>
+        <v>1822083.25427918</v>
       </c>
       <c r="D7" t="n">
-        <v>1014171.95913387</v>
+        <v>1011976.91399483</v>
       </c>
       <c r="E7" t="n">
-        <v>149681.809455467</v>
+        <v>149356.419004458</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>14078498.4685961</v>
+        <v>14054748.9659712</v>
       </c>
       <c r="B8" t="n">
-        <v>324862.629503348</v>
+        <v>324288.955167319</v>
       </c>
       <c r="C8" t="n">
-        <v>2645780.75324848</v>
+        <v>2641101.31926826</v>
       </c>
       <c r="D8" t="n">
-        <v>2020443.87605183</v>
+        <v>2016715.50047443</v>
       </c>
       <c r="E8" t="n">
-        <v>302429.087259049</v>
+        <v>301894.301637198</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>34878133.0241583</v>
+        <v>34839684.7187566</v>
       </c>
       <c r="B9" t="n">
-        <v>501328.365687305</v>
+        <v>500779.511466371</v>
       </c>
       <c r="C9" t="n">
-        <v>2692462.71860396</v>
+        <v>2689519.094084</v>
       </c>
       <c r="D9" t="n">
-        <v>1947508.64615275</v>
+        <v>1945368.91284485</v>
       </c>
       <c r="E9" t="n">
-        <v>1054082.32010245</v>
+        <v>1052934.4610938</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7003659.28667638</v>
+        <v>6978106.78391428</v>
       </c>
       <c r="B10" t="n">
-        <v>539249.518364065</v>
+        <v>537293.524485273</v>
       </c>
       <c r="C10" t="n">
-        <v>3671301.03572727</v>
+        <v>3658033.57277617</v>
       </c>
       <c r="D10" t="n">
-        <v>2003396.7265934</v>
+        <v>1996100.30105441</v>
       </c>
       <c r="E10" t="n">
-        <v>1781022.44594941</v>
+        <v>1774596.39223902</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2145321.42053728</v>
+        <v>2132286.57831435</v>
       </c>
       <c r="B11" t="n">
-        <v>304421.598260814</v>
+        <v>302589.307143644</v>
       </c>
       <c r="C11" t="n">
-        <v>1477367.38617365</v>
+        <v>1468384.33686602</v>
       </c>
       <c r="D11" t="n">
-        <v>1785327.18479696</v>
+        <v>1774534.94729985</v>
       </c>
       <c r="E11" t="n">
-        <v>132561.71693787</v>
+        <v>131748.183637641</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>420240.076795362</v>
+        <v>410486.629382001</v>
       </c>
       <c r="B12" t="n">
-        <v>65071.2259801104</v>
+        <v>63552.9693744729</v>
       </c>
       <c r="C12" t="n">
-        <v>700666.286564297</v>
+        <v>684258.617348153</v>
       </c>
       <c r="D12" t="n">
-        <v>806411.194926275</v>
+        <v>787541.574479678</v>
       </c>
       <c r="E12" t="n">
-        <v>64927.2782021999</v>
+        <v>63411.4137197223</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5065893.1726431</v>
+        <v>5061353.08751245</v>
       </c>
       <c r="B13" t="n">
-        <v>247806.123795423</v>
+        <v>247579.73043427</v>
       </c>
       <c r="C13" t="n">
-        <v>1476006.14699816</v>
+        <v>1474643.47703464</v>
       </c>
       <c r="D13" t="n">
-        <v>1505614.34362372</v>
+        <v>1504237.23137392</v>
       </c>
       <c r="E13" t="n">
-        <v>66812.5083491912</v>
+        <v>66751.5754326392</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>16234249.8352992</v>
+        <v>16219630.7095265</v>
       </c>
       <c r="B14" t="n">
-        <v>112761.78054877</v>
+        <v>112656.701626194</v>
       </c>
       <c r="C14" t="n">
-        <v>3214139.32622998</v>
+        <v>3211149.76213745</v>
       </c>
       <c r="D14" t="n">
-        <v>2240798.1651051</v>
+        <v>2238670.98418535</v>
       </c>
       <c r="E14" t="n">
-        <v>526054.544273636</v>
+        <v>525564.69413777</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3559486.64589327</v>
+        <v>3545332.45798819</v>
       </c>
       <c r="B15" t="n">
-        <v>158113.924112269</v>
+        <v>157449.670692812</v>
       </c>
       <c r="C15" t="n">
-        <v>3214688.7985411</v>
+        <v>3200600.08533833</v>
       </c>
       <c r="D15" t="n">
-        <v>1712113.45470886</v>
+        <v>1704895.44771509</v>
       </c>
       <c r="E15" t="n">
-        <v>621318.27182836</v>
+        <v>618700.618801889</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1681156.46552872</v>
+        <v>1675472.25234524</v>
       </c>
       <c r="B16" t="n">
-        <v>235715.093353867</v>
+        <v>234915.33421092</v>
       </c>
       <c r="C16" t="n">
-        <v>2922724.93887789</v>
+        <v>2912820.42187915</v>
       </c>
       <c r="D16" t="n">
-        <v>3008405.53962161</v>
+        <v>2998167.00954028</v>
       </c>
       <c r="E16" t="n">
-        <v>431161.911898409</v>
+        <v>429697.412521369</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>7931578.84841227</v>
+        <v>7919094.21678187</v>
       </c>
       <c r="B17" t="n">
-        <v>1112500.92145264</v>
+        <v>1110702.15455145</v>
       </c>
       <c r="C17" t="n">
-        <v>2260449.38093279</v>
+        <v>2256809.79937484</v>
       </c>
       <c r="D17" t="n">
-        <v>2081790.93908957</v>
+        <v>2078292.47349717</v>
       </c>
       <c r="E17" t="n">
-        <v>97278.8366899547</v>
+        <v>97115.0150339725</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>24937115.1041698</v>
+        <v>24927042.4588775</v>
       </c>
       <c r="B18" t="n">
-        <v>1620843.76431685</v>
+        <v>1620186.93878667</v>
       </c>
       <c r="C18" t="n">
-        <v>2827746.98262643</v>
+        <v>2826605.63318602</v>
       </c>
       <c r="D18" t="n">
-        <v>2580915.90534677</v>
+        <v>2579853.17023235</v>
       </c>
       <c r="E18" t="n">
-        <v>2287633.23591031</v>
+        <v>2286731.62087164</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>37969247.2962045</v>
+        <v>37931680.0581237</v>
       </c>
       <c r="B19" t="n">
-        <v>856510.290519298</v>
+        <v>855660.862410914</v>
       </c>
       <c r="C19" t="n">
-        <v>5085093.5341718</v>
+        <v>5080050.2980192</v>
       </c>
       <c r="D19" t="n">
-        <v>3453144.37309442</v>
+        <v>3449719.40688078</v>
       </c>
       <c r="E19" t="n">
-        <v>4647205.02337268</v>
+        <v>4642573.2401049</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>6913579.68542921</v>
+        <v>6901353.48732041</v>
       </c>
       <c r="B20" t="n">
-        <v>668417.737931854</v>
+        <v>667234.697527366</v>
       </c>
       <c r="C20" t="n">
-        <v>8772353.95466183</v>
+        <v>8756831.23675675</v>
       </c>
       <c r="D20" t="n">
-        <v>4650022.45978991</v>
+        <v>4641785.16299852</v>
       </c>
       <c r="E20" t="n">
-        <v>4085460.84180879</v>
+        <v>4078237.47699057</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2822975.42396008</v>
+        <v>2811875.1392604</v>
       </c>
       <c r="B21" t="n">
-        <v>1350888.30386219</v>
+        <v>1345575.81983853</v>
       </c>
       <c r="C21" t="n">
-        <v>4679207.93688917</v>
+        <v>4660805.78691372</v>
       </c>
       <c r="D21" t="n">
-        <v>3799977.7572537</v>
+        <v>3785029.67629515</v>
       </c>
       <c r="E21" t="n">
-        <v>2693245.71438962</v>
+        <v>2682649.72572253</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21513202.3880361</v>
+        <v>21496871.5596818</v>
       </c>
       <c r="B22" t="n">
-        <v>2666599.39798585</v>
+        <v>2664575.17770877</v>
       </c>
       <c r="C22" t="n">
-        <v>3310777.45950652</v>
+        <v>3308264.24853855</v>
       </c>
       <c r="D22" t="n">
-        <v>8452725.14417481</v>
+        <v>8446307.46046785</v>
       </c>
       <c r="E22" t="n">
-        <v>4151598.84215846</v>
+        <v>4148448.41716797</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>23937981.4808382</v>
+        <v>23930917.9599764</v>
       </c>
       <c r="B23" t="n">
-        <v>1193599.29195913</v>
+        <v>1193249.44310125</v>
       </c>
       <c r="C23" t="n">
-        <v>3877482.60582313</v>
+        <v>3876353.26551068</v>
       </c>
       <c r="D23" t="n">
-        <v>5460022.6629682</v>
+        <v>5458425.15902747</v>
       </c>
       <c r="E23" t="n">
-        <v>4168211.62738749</v>
+        <v>4166991.72248019</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>14098780.0791559</v>
+        <v>14093497.2877096</v>
       </c>
       <c r="B24" t="n">
-        <v>843891.12080947</v>
+        <v>843580.108842839</v>
       </c>
       <c r="C24" t="n">
-        <v>4238897.82489469</v>
+        <v>4237309.74534631</v>
       </c>
       <c r="D24" t="n">
-        <v>8334801.3357852</v>
+        <v>8331666.15506053</v>
       </c>
       <c r="E24" t="n">
-        <v>7943783.94185205</v>
+        <v>7940798.198577</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2013391.60809221</v>
+        <v>2012448.61147467</v>
       </c>
       <c r="B25" t="n">
-        <v>1021427.19851152</v>
+        <v>1020938.70833192</v>
       </c>
       <c r="C25" t="n">
-        <v>3993236.25858279</v>
+        <v>3991315.6478099</v>
       </c>
       <c r="D25" t="n">
-        <v>5509121.1431823</v>
+        <v>5506500.13181824</v>
       </c>
       <c r="E25" t="n">
-        <v>6730485.79280203</v>
+        <v>6727273.69630838</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>10324847.3734517</v>
+        <v>10318113.2555109</v>
       </c>
       <c r="B26" t="n">
-        <v>781226.113508079</v>
+        <v>780737.319047664</v>
       </c>
       <c r="C26" t="n">
-        <v>2320545.78678051</v>
+        <v>2319010.0769532</v>
       </c>
       <c r="D26" t="n">
-        <v>6389542.27700066</v>
+        <v>6385229.44375699</v>
       </c>
       <c r="E26" t="n">
-        <v>2911975.00044173</v>
+        <v>2910012.70740262</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>6869071.66343605</v>
+        <v>6860048.61303467</v>
       </c>
       <c r="B27" t="n">
-        <v>852208.579977773</v>
+        <v>851134.598508383</v>
       </c>
       <c r="C27" t="n">
-        <v>1965531.59517291</v>
+        <v>1962972.63405864</v>
       </c>
       <c r="D27" t="n">
-        <v>8128447.49462448</v>
+        <v>8117564.37841504</v>
       </c>
       <c r="E27" t="n">
-        <v>2158033.31781319</v>
+        <v>2155143.21173209</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>20487155.0884189</v>
+        <v>20484407.9990749</v>
       </c>
       <c r="B28" t="n">
-        <v>1379536.78960042</v>
+        <v>1379369.76643916</v>
       </c>
       <c r="C28" t="n">
-        <v>3670318.3435436</v>
+        <v>3669831.29570439</v>
       </c>
       <c r="D28" t="n">
-        <v>9808816.23790985</v>
+        <v>9807459.99294916</v>
       </c>
       <c r="E28" t="n">
-        <v>5364082.17208796</v>
+        <v>5363340.07177571</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>18196239.6555184</v>
+        <v>18192988.9610095</v>
       </c>
       <c r="B29" t="n">
-        <v>1591683.26461317</v>
+        <v>1591425.18655397</v>
       </c>
       <c r="C29" t="n">
-        <v>8301845.45735842</v>
+        <v>8300331.60001511</v>
       </c>
       <c r="D29" t="n">
-        <v>12607774.2094124</v>
+        <v>12605427.2265248</v>
       </c>
       <c r="E29" t="n">
-        <v>2713122.25590398</v>
+        <v>2712617.43817658</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>8618838.95977736</v>
+        <v>8613126.79373104</v>
       </c>
       <c r="B30" t="n">
-        <v>1685749.56253567</v>
+        <v>1684654.87073035</v>
       </c>
       <c r="C30" t="n">
-        <v>9761107.26254106</v>
+        <v>9754424.63193796</v>
       </c>
       <c r="D30" t="n">
-        <v>9241844.78138794</v>
+        <v>9235470.32797002</v>
       </c>
       <c r="E30" t="n">
-        <v>5963146.65277959</v>
+        <v>5959036.39541095</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>10638380.6856266</v>
+        <v>10628639.80781</v>
       </c>
       <c r="B31" t="n">
-        <v>1462984.01638927</v>
+        <v>1461638.58583167</v>
       </c>
       <c r="C31" t="n">
-        <v>5227861.36828423</v>
+        <v>5222906.78433975</v>
       </c>
       <c r="D31" t="n">
-        <v>17908014.0000887</v>
+        <v>17890992.6670523</v>
       </c>
       <c r="E31" t="n">
-        <v>6347256.73453694</v>
+        <v>6341238.57209666</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>8070236.88492487</v>
+        <v>8064870.92930171</v>
       </c>
       <c r="B32" t="n">
-        <v>2453359.47972206</v>
+        <v>2451734.91460254</v>
       </c>
       <c r="C32" t="n">
-        <v>5580987.19194448</v>
+        <v>5577184.76230529</v>
       </c>
       <c r="D32" t="n">
-        <v>24267393.3327151</v>
+        <v>24250547.8661022</v>
       </c>
       <c r="E32" t="n">
-        <v>6221016.78607043</v>
+        <v>6216697.59077248</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>21598221.3514163</v>
+        <v>21592336.7811101</v>
       </c>
       <c r="B33" t="n">
-        <v>2062528.43061709</v>
+        <v>2062023.39957804</v>
       </c>
       <c r="C33" t="n">
-        <v>3701770.10595001</v>
+        <v>3700808.24099731</v>
       </c>
       <c r="D33" t="n">
-        <v>12741855.8931461</v>
+        <v>12738312.48119</v>
       </c>
       <c r="E33" t="n">
-        <v>5571512.63717274</v>
+        <v>5569971.24474242</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>28438260.3563645</v>
+        <v>28426663.0920155</v>
       </c>
       <c r="B34" t="n">
-        <v>2199590.75215272</v>
+        <v>2198777.94095593</v>
       </c>
       <c r="C34" t="n">
-        <v>3441484.28622961</v>
+        <v>3440141.64366799</v>
       </c>
       <c r="D34" t="n">
-        <v>15381379.1258489</v>
+        <v>15374929.5365239</v>
       </c>
       <c r="E34" t="n">
-        <v>5915436.42004549</v>
+        <v>5912957.99819856</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>4476424.07254114</v>
+        <v>4474670.18709662</v>
       </c>
       <c r="B35" t="n">
-        <v>2384506.72883278</v>
+        <v>2383541.73485249</v>
       </c>
       <c r="C35" t="n">
-        <v>4664365.90819997</v>
+        <v>4662460.92687805</v>
       </c>
       <c r="D35" t="n">
-        <v>12421294.6983441</v>
+        <v>12416197.4084332</v>
       </c>
       <c r="E35" t="n">
-        <v>5372854.2239083</v>
+        <v>5370652.68041035</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2394495.22293921</v>
+        <v>2392217.58377671</v>
       </c>
       <c r="B36" t="n">
-        <v>815108.24901881</v>
+        <v>814336.197878363</v>
       </c>
       <c r="C36" t="n">
-        <v>1912475.1486488</v>
+        <v>1910810.19554351</v>
       </c>
       <c r="D36" t="n">
-        <v>7939769.05004735</v>
+        <v>7932122.5109884</v>
       </c>
       <c r="E36" t="n">
-        <v>2511164.36232858</v>
+        <v>2508751.34817347</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>3814636.35209901</v>
+        <v>3811020.54933579</v>
       </c>
       <c r="B37" t="n">
-        <v>1186727.89054117</v>
+        <v>1185591.3032878</v>
       </c>
       <c r="C37" t="n">
-        <v>2367415.48416162</v>
+        <v>2365116.31797275</v>
       </c>
       <c r="D37" t="n">
-        <v>4694215.9739727</v>
+        <v>4689597.35076699</v>
       </c>
       <c r="E37" t="n">
-        <v>1894134.52334231</v>
+        <v>1892274.61802163</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>13209434.1763576</v>
+        <v>13203151.60731</v>
       </c>
       <c r="B38" t="n">
-        <v>3030356.39827223</v>
+        <v>3028936.65018383</v>
       </c>
       <c r="C38" t="n">
-        <v>4703671.75852375</v>
+        <v>4701483.59076066</v>
       </c>
       <c r="D38" t="n">
-        <v>6484251.04453313</v>
+        <v>6481074.18857498</v>
       </c>
       <c r="E38" t="n">
-        <v>5226446.07882312</v>
+        <v>5223880.80698123</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3576457.04635078</v>
+        <v>3569954.42189217</v>
       </c>
       <c r="B39" t="n">
-        <v>2193206.05792903</v>
+        <v>2189166.18180026</v>
       </c>
       <c r="C39" t="n">
-        <v>3973176.72266005</v>
+        <v>3967395.19737614</v>
       </c>
       <c r="D39" t="n">
-        <v>8184338.16581621</v>
+        <v>8168698.91105065</v>
       </c>
       <c r="E39" t="n">
-        <v>2304489.96904735</v>
+        <v>2300098.25586632</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1941024.12731513</v>
+        <v>1940224.70789801</v>
       </c>
       <c r="B40" t="n">
-        <v>1187400.27976896</v>
+        <v>1186912.55500454</v>
       </c>
       <c r="C40" t="n">
-        <v>5992710.06015729</v>
+        <v>5991184.94011636</v>
       </c>
       <c r="D40" t="n">
-        <v>3568069.47588067</v>
+        <v>3566444.17863823</v>
       </c>
       <c r="E40" t="n">
-        <v>1468239.85527438</v>
+        <v>1467574.96236237</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>898652.997928252</v>
+        <v>897873.610995055</v>
       </c>
       <c r="B41" t="n">
-        <v>942136.692138607</v>
+        <v>941300.532883602</v>
       </c>
       <c r="C41" t="n">
-        <v>2815062.38762195</v>
+        <v>2813597.6573911</v>
       </c>
       <c r="D41" t="n">
-        <v>5549531.26500982</v>
+        <v>5544321.67353937</v>
       </c>
       <c r="E41" t="n">
-        <v>2501399.69034325</v>
+        <v>2499048.61206048</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2003165.36919968</v>
+        <v>2001774.82342509</v>
       </c>
       <c r="B42" t="n">
-        <v>4160779.04704635</v>
+        <v>4157785.6451067</v>
       </c>
       <c r="C42" t="n">
-        <v>4863197.71219149</v>
+        <v>4861575.06955801</v>
       </c>
       <c r="D42" t="n">
-        <v>3219849.60706623</v>
+        <v>3217355.09958705</v>
       </c>
       <c r="E42" t="n">
-        <v>2542168.32626273</v>
+        <v>2540239.58304044</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>8094074.74771298</v>
+        <v>8091208.1666172</v>
       </c>
       <c r="B43" t="n">
-        <v>7528554.52078045</v>
+        <v>7525883.78592674</v>
       </c>
       <c r="C43" t="n">
-        <v>4067811.80765356</v>
+        <v>4066682.05979442</v>
       </c>
       <c r="D43" t="n">
-        <v>11646819.659362</v>
+        <v>11642565.1686825</v>
       </c>
       <c r="E43" t="n">
-        <v>4204326.57969453</v>
+        <v>4202790.67246846</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2868899.93990473</v>
+        <v>2867678.88833906</v>
       </c>
       <c r="B44" t="n">
-        <v>5226969.46989292</v>
+        <v>5224715.57942629</v>
       </c>
       <c r="C44" t="n">
-        <v>8767576.41028184</v>
+        <v>8765371.00209191</v>
       </c>
       <c r="D44" t="n">
-        <v>9406629.26161336</v>
+        <v>9402204.39316822</v>
       </c>
       <c r="E44" t="n">
-        <v>3091463.44108508</v>
+        <v>3090001.95045515</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>5718220.42331093</v>
+        <v>5715389.79540332</v>
       </c>
       <c r="B45" t="n">
-        <v>3344495.45457376</v>
+        <v>3342878.91699753</v>
       </c>
       <c r="C45" t="n">
-        <v>5343867.98083382</v>
+        <v>5342241.08517527</v>
       </c>
       <c r="D45" t="n">
-        <v>8618257.55986788</v>
+        <v>8613841.9371439</v>
       </c>
       <c r="E45" t="n">
-        <v>3781119.87656948</v>
+        <v>3779176.12739619</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>5922721.13593924</v>
+        <v>5917491.96398382</v>
       </c>
       <c r="B46" t="n">
-        <v>4775528.62579642</v>
+        <v>4771232.68329985</v>
       </c>
       <c r="C46" t="n">
-        <v>8443878.0900208</v>
+        <v>8438491.67681472</v>
       </c>
       <c r="D46" t="n">
-        <v>7402410.79748568</v>
+        <v>7395032.41651541</v>
       </c>
       <c r="E46" t="n">
-        <v>7407077.31694388</v>
+        <v>7399703.24631616</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>6035713.38157724</v>
+        <v>6030619.59934621</v>
       </c>
       <c r="B47" t="n">
-        <v>4708633.53347139</v>
+        <v>4704660.31156615</v>
       </c>
       <c r="C47" t="n">
-        <v>9135283.59323284</v>
+        <v>9127187.81145795</v>
       </c>
       <c r="D47" t="n">
-        <v>7832260.39546563</v>
+        <v>7825252.25167802</v>
       </c>
       <c r="E47" t="n">
-        <v>2932522.44116378</v>
+        <v>2929894.71021366</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>6965720.45875378</v>
+        <v>6961784.0943185</v>
       </c>
       <c r="B48" t="n">
-        <v>2370583.74147279</v>
+        <v>2369159.92903797</v>
       </c>
       <c r="C48" t="n">
-        <v>4915957.28460135</v>
+        <v>4912919.86151694</v>
       </c>
       <c r="D48" t="n">
-        <v>12277307.7716419</v>
+        <v>12269670.949551</v>
       </c>
       <c r="E48" t="n">
-        <v>3853654.20695234</v>
+        <v>3851254.22256373</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>10783500.1076204</v>
+        <v>10779329.0658282</v>
       </c>
       <c r="B49" t="n">
-        <v>2816626.73968034</v>
+        <v>2815554.25685875</v>
       </c>
       <c r="C49" t="n">
-        <v>5439048.99673172</v>
+        <v>5436897.89915507</v>
       </c>
       <c r="D49" t="n">
-        <v>5147758.72933031</v>
+        <v>5145650.23575105</v>
       </c>
       <c r="E49" t="n">
-        <v>4990784.0686803</v>
+        <v>4988743.50015311</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>7236986.66397184</v>
+        <v>7228364.43835473</v>
       </c>
       <c r="B50" t="n">
-        <v>2251976.5380423</v>
+        <v>2249301.67131854</v>
       </c>
       <c r="C50" t="n">
-        <v>5526913.81294431</v>
+        <v>5520113.23052997</v>
       </c>
       <c r="D50" t="n">
-        <v>4609984.46105266</v>
+        <v>4604185.01717166</v>
       </c>
       <c r="E50" t="n">
-        <v>4208695.0539786</v>
+        <v>4203387.32751037</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>12281202.4238118</v>
+        <v>12263918.5884778</v>
       </c>
       <c r="B51" t="n">
-        <v>2229563.97802948</v>
+        <v>2226527.14824683</v>
       </c>
       <c r="C51" t="n">
-        <v>3326198.39385591</v>
+        <v>3321536.1437245</v>
       </c>
       <c r="D51" t="n">
-        <v>5931750.74545945</v>
+        <v>5923046.40444792</v>
       </c>
       <c r="E51" t="n">
-        <v>2925111.46190956</v>
+        <v>2920818.01974628</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>6334062.70682489</v>
+        <v>6324295.12249529</v>
       </c>
       <c r="B52" t="n">
-        <v>1932716.58836887</v>
+        <v>1929766.92738698</v>
       </c>
       <c r="C52" t="n">
-        <v>3078915.53905401</v>
+        <v>3074128.06890756</v>
       </c>
       <c r="D52" t="n">
-        <v>5132660.24604262</v>
+        <v>5124465.51224934</v>
       </c>
       <c r="E52" t="n">
-        <v>2637889.97559458</v>
+        <v>2633700.23176688</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>17604153.1422118</v>
+        <v>17600068.1867043</v>
       </c>
       <c r="B53" t="n">
-        <v>1620613.92667215</v>
+        <v>1620274.25102924</v>
       </c>
       <c r="C53" t="n">
-        <v>5321533.51511964</v>
+        <v>5320300.43306575</v>
       </c>
       <c r="D53" t="n">
-        <v>5079722.69255457</v>
+        <v>5078503.21443077</v>
       </c>
       <c r="E53" t="n">
-        <v>1154294.10978984</v>
+        <v>1154016.58071865</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>23109434.6438371</v>
+        <v>23104927.301169</v>
       </c>
       <c r="B54" t="n">
-        <v>8246125.3717252</v>
+        <v>8244526.01632921</v>
       </c>
       <c r="C54" t="n">
-        <v>6091921.89574901</v>
+        <v>6090738.02933237</v>
       </c>
       <c r="D54" t="n">
-        <v>8509714.53506543</v>
+        <v>8508004.37541159</v>
       </c>
       <c r="E54" t="n">
-        <v>4249912.1560737</v>
+        <v>4249070.2718959</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>14202028.9615466</v>
+        <v>14196138.4617503</v>
       </c>
       <c r="B55" t="n">
-        <v>4940402.17111843</v>
+        <v>4938325.4775034</v>
       </c>
       <c r="C55" t="n">
-        <v>5039292.61341431</v>
+        <v>5037142.32421392</v>
       </c>
       <c r="D55" t="n">
-        <v>9896198.18793987</v>
+        <v>9891849.56228362</v>
       </c>
       <c r="E55" t="n">
-        <v>7195957.00076874</v>
+        <v>7192817.67980257</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>7253416.68148115</v>
+        <v>7250329.62986299</v>
       </c>
       <c r="B56" t="n">
-        <v>4432243.41447829</v>
+        <v>4430315.48637172</v>
       </c>
       <c r="C56" t="n">
-        <v>5978321.35469949</v>
+        <v>5975665.58016024</v>
       </c>
       <c r="D56" t="n">
-        <v>12446850.5786484</v>
+        <v>12441095.3321744</v>
       </c>
       <c r="E56" t="n">
-        <v>6675812.24388054</v>
+        <v>6672737.54141067</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>7232365.00984057</v>
+        <v>7466678.17076632</v>
       </c>
       <c r="B57" t="n">
-        <v>2992428.51556573</v>
+        <v>2873548.83069059</v>
       </c>
       <c r="C57" t="n">
-        <v>6839001.18983133</v>
+        <v>6926059.93262777</v>
       </c>
       <c r="D57" t="n">
-        <v>6560205.10870885</v>
+        <v>6104311.05201962</v>
       </c>
       <c r="E57" t="n">
-        <v>4513683.34761873</v>
+        <v>4770221.93813868</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>7894832.33911682</v>
+        <v>7915105.99037233</v>
       </c>
       <c r="B58" t="n">
-        <v>1846733.69554717</v>
+        <v>1850421.2031931</v>
       </c>
       <c r="C58" t="n">
-        <v>8803660.57998771</v>
+        <v>8808239.41971106</v>
       </c>
       <c r="D58" t="n">
-        <v>15504272.5568979</v>
+        <v>15431958.9920806</v>
       </c>
       <c r="E58" t="n">
-        <v>3571567.30924299</v>
+        <v>3604497.65166551</v>
       </c>
     </row>
   </sheetData>
@@ -4315,36 +4315,36 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>7143363.67197492</v>
+        <v>7373322.83317892</v>
       </c>
       <c r="B57" t="n">
-        <v>2951434.65166409</v>
+        <v>2835628.99208836</v>
       </c>
       <c r="C57" t="n">
-        <v>6771836.31403837</v>
+        <v>6855362.76479903</v>
       </c>
       <c r="D57" t="n">
-        <v>6475407.74121258</v>
+        <v>6022540.80942736</v>
       </c>
       <c r="E57" t="n">
-        <v>4450533.52447565</v>
+        <v>4705720.6427068</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>7815360.16747234</v>
+        <v>7837003.14208972</v>
       </c>
       <c r="B58" t="n">
-        <v>1827934.84282681</v>
+        <v>1832020.7460117</v>
       </c>
       <c r="C58" t="n">
-        <v>8715501.89620838</v>
+        <v>8721876.61986984</v>
       </c>
       <c r="D58" t="n">
-        <v>15317041.5988176</v>
+        <v>15251370.6144035</v>
       </c>
       <c r="E58" t="n">
-        <v>3528880.7549855</v>
+        <v>3562448.09452901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated output for 2020 run reconstruction
</commit_message>
<xml_diff>
--- a/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
+++ b/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
@@ -1347,6 +1347,23 @@
         <v>1543355.63842831</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>4028889.48167101</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2385881.40802501</v>
+      </c>
+      <c r="C59" t="n">
+        <v>4110477.96951001</v>
+      </c>
+      <c r="D59" t="n">
+        <v>2412280.997283</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1732176.2079256</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2315,36 +2332,53 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>3067970.1707458</v>
+        <v>3067971.65104639</v>
       </c>
       <c r="B57" t="n">
-        <v>1292122.83030637</v>
+        <v>1292123.43158704</v>
       </c>
       <c r="C57" t="n">
-        <v>4704907.93181197</v>
+        <v>4704909.05283045</v>
       </c>
       <c r="D57" t="n">
-        <v>4495954.05218515</v>
+        <v>4495955.34878523</v>
       </c>
       <c r="E57" t="n">
-        <v>3602429.93779496</v>
+        <v>3602430.96056782</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>5543863.9901118</v>
+        <v>5565069.48341984</v>
       </c>
       <c r="B58" t="n">
-        <v>1029963.20319573</v>
+        <v>1034687.52937156</v>
       </c>
       <c r="C58" t="n">
-        <v>5896769.41891236</v>
+        <v>5913187.20470384</v>
       </c>
       <c r="D58" t="n">
-        <v>13091748.9829389</v>
+        <v>13093842.4110679</v>
       </c>
       <c r="E58" t="n">
-        <v>2056749.6512372</v>
+        <v>2057215.09245664</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>5944787.03766096</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2227286.75334413</v>
+      </c>
+      <c r="C59" t="n">
+        <v>6101073.0695064</v>
+      </c>
+      <c r="D59" t="n">
+        <v>13404240.0411759</v>
+      </c>
+      <c r="E59" t="n">
+        <v>3396471.7587296</v>
       </c>
     </row>
   </sheetData>
@@ -3315,36 +3349,53 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>7466678.17076632</v>
+        <v>7466679.6510669</v>
       </c>
       <c r="B57" t="n">
-        <v>2873548.83069059</v>
+        <v>2873549.43197125</v>
       </c>
       <c r="C57" t="n">
-        <v>6926059.93262777</v>
+        <v>6926061.05364625</v>
       </c>
       <c r="D57" t="n">
-        <v>6104311.05201962</v>
+        <v>6104312.34861969</v>
       </c>
       <c r="E57" t="n">
-        <v>4770221.93813868</v>
+        <v>4770222.96091154</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>7915105.99037233</v>
+        <v>7936311.48368038</v>
       </c>
       <c r="B58" t="n">
-        <v>1850421.2031931</v>
+        <v>1855145.52936893</v>
       </c>
       <c r="C58" t="n">
-        <v>8808239.41971106</v>
+        <v>8824657.20550253</v>
       </c>
       <c r="D58" t="n">
-        <v>15431958.9920806</v>
+        <v>15434052.4202096</v>
       </c>
       <c r="E58" t="n">
-        <v>3604497.65166551</v>
+        <v>3604963.09288495</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>9975755.03733196</v>
+      </c>
+      <c r="B59" t="n">
+        <v>4613804.75336914</v>
+      </c>
+      <c r="C59" t="n">
+        <v>10213233.0700164</v>
+      </c>
+      <c r="D59" t="n">
+        <v>15793968.0414589</v>
+      </c>
+      <c r="E59" t="n">
+        <v>5142411.7586552</v>
       </c>
     </row>
   </sheetData>
@@ -4332,19 +4383,36 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>7837003.14208972</v>
+        <v>7857381.16684172</v>
       </c>
       <c r="B58" t="n">
-        <v>1832020.7460117</v>
+        <v>1836550.1266757</v>
       </c>
       <c r="C58" t="n">
-        <v>8721876.61986984</v>
+        <v>8737379.42620984</v>
       </c>
       <c r="D58" t="n">
-        <v>15251370.6144035</v>
+        <v>15251550.7806298</v>
       </c>
       <c r="E58" t="n">
-        <v>3562448.09452901</v>
+        <v>3562468.037446</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>9811353.21886345</v>
+      </c>
+      <c r="B59" t="n">
+        <v>4534935.15862568</v>
+      </c>
+      <c r="C59" t="n">
+        <v>10046645.3940871</v>
+      </c>
+      <c r="D59" t="n">
+        <v>15501887.0430196</v>
+      </c>
+      <c r="E59" t="n">
+        <v>5047701.89071117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add all updated files and figures for 2021 reconstruction
</commit_message>
<xml_diff>
--- a/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
+++ b/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
@@ -1364,6 +1364,23 @@
         <v>1732176.2079256</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>4688089.278375</v>
+      </c>
+      <c r="B60" t="n">
+        <v>3230621.48119301</v>
+      </c>
+      <c r="C60" t="n">
+        <v>2780528.141222</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1849311.35638</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2902367.4527424</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -2366,19 +2383,36 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>5944787.03766096</v>
+        <v>5835696.59801433</v>
       </c>
       <c r="B59" t="n">
-        <v>2227286.75334413</v>
+        <v>2174689.96366779</v>
       </c>
       <c r="C59" t="n">
-        <v>6101073.0695064</v>
+        <v>5990051.95581967</v>
       </c>
       <c r="D59" t="n">
-        <v>13404240.0411759</v>
+        <v>13207490.5318939</v>
       </c>
       <c r="E59" t="n">
-        <v>3396471.7587296</v>
+        <v>3332673.97612231</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>4173540.65451519</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2824542.76335536</v>
+      </c>
+      <c r="C60" t="n">
+        <v>4315536.2001339</v>
+      </c>
+      <c r="D60" t="n">
+        <v>5885686.24853126</v>
+      </c>
+      <c r="E60" t="n">
+        <v>7805217.15984679</v>
       </c>
     </row>
   </sheetData>
@@ -3383,19 +3417,36 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>9975755.03733196</v>
+        <v>9866664.59768534</v>
       </c>
       <c r="B59" t="n">
-        <v>4613804.75336914</v>
+        <v>4561207.9636928</v>
       </c>
       <c r="C59" t="n">
-        <v>10213233.0700164</v>
+        <v>10102211.9563297</v>
       </c>
       <c r="D59" t="n">
-        <v>15793968.0414589</v>
+        <v>15597218.5321769</v>
       </c>
       <c r="E59" t="n">
-        <v>5142411.7586552</v>
+        <v>5078613.97604791</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>8877060.6548902</v>
+      </c>
+      <c r="B60" t="n">
+        <v>6061446.76354836</v>
+      </c>
+      <c r="C60" t="n">
+        <v>7112070.1993559</v>
+      </c>
+      <c r="D60" t="n">
+        <v>7717882.24891126</v>
+      </c>
+      <c r="E60" t="n">
+        <v>10665147.1595892</v>
       </c>
     </row>
   </sheetData>
@@ -4400,19 +4451,36 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>9811353.21886345</v>
+        <v>9813005.95416345</v>
       </c>
       <c r="B59" t="n">
-        <v>4534935.15862568</v>
+        <v>4535465.94022568</v>
       </c>
       <c r="C59" t="n">
-        <v>10046645.3940871</v>
+        <v>10047839.8769871</v>
       </c>
       <c r="D59" t="n">
         <v>15501887.0430196</v>
       </c>
       <c r="E59" t="n">
         <v>5047701.89071117</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>8453208.9993308</v>
+      </c>
+      <c r="B60" t="n">
+        <v>5768722.89931442</v>
+      </c>
+      <c r="C60" t="n">
+        <v>6801010.79850064</v>
+      </c>
+      <c r="D60" t="n">
+        <v>7315452.9239985</v>
+      </c>
+      <c r="E60" t="n">
+        <v>10108062.8180798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated final run for 2021, based on V1
</commit_message>
<xml_diff>
--- a/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
+++ b/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
@@ -1366,19 +1366,19 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>4688089.278375</v>
+        <v>4687888.21634433</v>
       </c>
       <c r="B60" t="n">
-        <v>3230621.48119301</v>
+        <v>3229999.83754533</v>
       </c>
       <c r="C60" t="n">
-        <v>2780528.141222</v>
+        <v>2783049.2461762</v>
       </c>
       <c r="D60" t="n">
-        <v>1849311.35638</v>
+        <v>1846975.3373724</v>
       </c>
       <c r="E60" t="n">
-        <v>2902367.4527424</v>
+        <v>2903009.95933991</v>
       </c>
     </row>
   </sheetData>
@@ -2400,19 +2400,19 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>4173540.65451519</v>
+        <v>4182270.2673438</v>
       </c>
       <c r="B60" t="n">
-        <v>2824542.76335536</v>
+        <v>2832609.70661295</v>
       </c>
       <c r="C60" t="n">
-        <v>4315536.2001339</v>
+        <v>4299080.64742782</v>
       </c>
       <c r="D60" t="n">
-        <v>5885686.24853126</v>
+        <v>5893351.00034585</v>
       </c>
       <c r="E60" t="n">
-        <v>7805217.15984679</v>
+        <v>7797211.51975421</v>
       </c>
     </row>
   </sheetData>
@@ -3434,19 +3434,19 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>8877060.6548902</v>
+        <v>8885790.26768812</v>
       </c>
       <c r="B60" t="n">
-        <v>6061446.76354836</v>
+        <v>6069513.70615829</v>
       </c>
       <c r="C60" t="n">
-        <v>7112070.1993559</v>
+        <v>7095614.64760402</v>
       </c>
       <c r="D60" t="n">
-        <v>7717882.24891126</v>
+        <v>7725547.00071825</v>
       </c>
       <c r="E60" t="n">
-        <v>10665147.1595892</v>
+        <v>10657141.5200941</v>
       </c>
     </row>
   </sheetData>
@@ -4468,19 +4468,19 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>8453208.9993308</v>
+        <v>8461494.92707114</v>
       </c>
       <c r="B60" t="n">
-        <v>5768722.89931442</v>
+        <v>5776402.50584379</v>
       </c>
       <c r="C60" t="n">
-        <v>6801010.79850064</v>
+        <v>6785280.23768978</v>
       </c>
       <c r="D60" t="n">
-        <v>7315452.9239985</v>
+        <v>7322840.46632597</v>
       </c>
       <c r="E60" t="n">
-        <v>10108062.8180798</v>
+        <v>10100440.3009972</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Syrah v1 run update Oct 2022
</commit_message>
<xml_diff>
--- a/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
+++ b/Syrah/outputFiles/EastSide Figs/Extras/Daniel Summary_east.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -354,12 +354,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1366,19 +1366,36 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>4687888.21634433</v>
+        <v>4699177.00994884</v>
       </c>
       <c r="B60" t="n">
-        <v>3229999.83754533</v>
+        <v>3235008.49876586</v>
       </c>
       <c r="C60" t="n">
-        <v>2783049.2461762</v>
+        <v>2791483.41477137</v>
       </c>
       <c r="D60" t="n">
-        <v>1846975.3373724</v>
+        <v>1843084.01158241</v>
       </c>
       <c r="E60" t="n">
-        <v>2903009.95933991</v>
+        <v>2862364.22598788</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>4216292.88421672</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1667776.76874747</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1919900.90466542</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1797726.02681772</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1434912.60671791</v>
       </c>
     </row>
   </sheetData>
@@ -1388,12 +1405,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -2094,36 +2111,36 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>314970.823885078</v>
+        <v>314970.90111517</v>
       </c>
       <c r="B42" t="n">
-        <v>481639.645227682</v>
+        <v>481639.811479459</v>
       </c>
       <c r="C42" t="n">
-        <v>3030405.06984201</v>
+        <v>3030405.15996262</v>
       </c>
       <c r="D42" t="n">
-        <v>2065235.09925069</v>
+        <v>2065235.23779417</v>
       </c>
       <c r="E42" t="n">
-        <v>1750037.5830476</v>
+        <v>1750037.69016886</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2591074.16575682</v>
+        <v>2591144.30901509</v>
       </c>
       <c r="B43" t="n">
-        <v>2129291.78554283</v>
+        <v>2129357.13657891</v>
       </c>
       <c r="C43" t="n">
-        <v>2127008.05990141</v>
+        <v>2127035.70405073</v>
       </c>
       <c r="D43" t="n">
-        <v>10352421.1683057</v>
+        <v>10352525.2727523</v>
       </c>
       <c r="E43" t="n">
-        <v>3387686.67258656</v>
+        <v>3387724.25517489</v>
       </c>
     </row>
     <row r="44">
@@ -2179,19 +2196,19 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>3272707.5986842</v>
+        <v>3274439.80359764</v>
       </c>
       <c r="B47" t="n">
-        <v>2524158.31143013</v>
+        <v>2525509.45566722</v>
       </c>
       <c r="C47" t="n">
-        <v>6654497.81083594</v>
+        <v>6657250.88356904</v>
       </c>
       <c r="D47" t="n">
-        <v>6565684.25146314</v>
+        <v>6568067.45917646</v>
       </c>
       <c r="E47" t="n">
-        <v>2333562.71027486</v>
+        <v>2334456.30333726</v>
       </c>
     </row>
     <row r="48">
@@ -2247,70 +2264,70 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>8099474.58931948</v>
+        <v>8104598.28359105</v>
       </c>
       <c r="B51" t="n">
-        <v>1364780.14818682</v>
+        <v>1365680.39903163</v>
       </c>
       <c r="C51" t="n">
-        <v>2421224.1436332</v>
+        <v>2422606.24105714</v>
       </c>
       <c r="D51" t="n">
-        <v>4689146.40433662</v>
+        <v>4691726.75651637</v>
       </c>
       <c r="E51" t="n">
-        <v>2225800.01970357</v>
+        <v>2227072.78611174</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>4235719.12242102</v>
+        <v>4237256.55138693</v>
       </c>
       <c r="B52" t="n">
-        <v>833816.927896934</v>
+        <v>834281.207915428</v>
       </c>
       <c r="C52" t="n">
-        <v>2135968.06887827</v>
+        <v>2136721.62216516</v>
       </c>
       <c r="D52" t="n">
-        <v>4010835.51229691</v>
+        <v>4012125.37278612</v>
       </c>
       <c r="E52" t="n">
-        <v>1735590.23183467</v>
+        <v>1736249.70231408</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>13141528.1867971</v>
+        <v>13150933.7372542</v>
       </c>
       <c r="B53" t="n">
-        <v>1419774.25104763</v>
+        <v>1420556.34925961</v>
       </c>
       <c r="C53" t="n">
-        <v>3845872.43272374</v>
+        <v>3848711.58616231</v>
       </c>
       <c r="D53" t="n">
-        <v>3696037.21468247</v>
+        <v>3698845.04527047</v>
       </c>
       <c r="E53" t="n">
-        <v>513858.58068414</v>
+        <v>514497.587321458</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>15763315.3012893</v>
+        <v>15762177.6874716</v>
       </c>
       <c r="B54" t="n">
-        <v>2473876.01750705</v>
+        <v>2473472.35421099</v>
       </c>
       <c r="C54" t="n">
-        <v>4169784.02921601</v>
+        <v>4169485.23169982</v>
       </c>
       <c r="D54" t="n">
-        <v>6347212.37502937</v>
+        <v>6346780.74570896</v>
       </c>
       <c r="E54" t="n">
-        <v>2684432.27201083</v>
+        <v>2684219.78781691</v>
       </c>
     </row>
     <row r="55">
@@ -2400,19 +2417,36 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>4182270.2673438</v>
+        <v>4203779.85155197</v>
       </c>
       <c r="B60" t="n">
-        <v>2832609.70661295</v>
+        <v>2887384.46275631</v>
       </c>
       <c r="C60" t="n">
-        <v>4299080.64742782</v>
+        <v>4383754.52775887</v>
       </c>
       <c r="D60" t="n">
-        <v>5893351.00034585</v>
+        <v>5536043.36492513</v>
       </c>
       <c r="E60" t="n">
-        <v>7797211.51975421</v>
+        <v>8000213.50067119</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>9467949.67417201</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2992284.52106209</v>
+      </c>
+      <c r="C61" t="n">
+        <v>4553748.84846504</v>
+      </c>
+      <c r="D61" t="n">
+        <v>16433879.5528658</v>
+      </c>
+      <c r="E61" t="n">
+        <v>6123276.48256126</v>
       </c>
     </row>
   </sheetData>
@@ -2422,12 +2456,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -3128,36 +3162,36 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2001774.82342509</v>
+        <v>2001774.90065518</v>
       </c>
       <c r="B42" t="n">
-        <v>4157785.6451067</v>
+        <v>4157785.81135847</v>
       </c>
       <c r="C42" t="n">
-        <v>4861575.06955801</v>
+        <v>4861575.15967863</v>
       </c>
       <c r="D42" t="n">
-        <v>3217355.09958705</v>
+        <v>3217355.23813052</v>
       </c>
       <c r="E42" t="n">
-        <v>2540239.58304044</v>
+        <v>2540239.6901617</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>8091208.1666172</v>
+        <v>8091278.30987547</v>
       </c>
       <c r="B43" t="n">
-        <v>7525883.78592674</v>
+        <v>7525949.13696282</v>
       </c>
       <c r="C43" t="n">
-        <v>4066682.05979442</v>
+        <v>4066709.70394374</v>
       </c>
       <c r="D43" t="n">
-        <v>11642565.1686825</v>
+        <v>11642669.2731291</v>
       </c>
       <c r="E43" t="n">
-        <v>4202790.67246846</v>
+        <v>4202828.25505679</v>
       </c>
     </row>
     <row r="44">
@@ -3213,19 +3247,19 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>6030619.59934621</v>
+        <v>6032351.80425965</v>
       </c>
       <c r="B47" t="n">
-        <v>4704660.31156615</v>
+        <v>4706011.45580324</v>
       </c>
       <c r="C47" t="n">
-        <v>9127187.81145795</v>
+        <v>9129940.88419104</v>
       </c>
       <c r="D47" t="n">
-        <v>7825252.25167802</v>
+        <v>7827635.45939134</v>
       </c>
       <c r="E47" t="n">
-        <v>2929894.71021366</v>
+        <v>2930788.30327605</v>
       </c>
     </row>
     <row r="48">
@@ -3281,70 +3315,70 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>12263918.5884778</v>
+        <v>12269042.2827494</v>
       </c>
       <c r="B51" t="n">
-        <v>2226527.14824683</v>
+        <v>2227427.39909164</v>
       </c>
       <c r="C51" t="n">
-        <v>3321536.1437245</v>
+        <v>3322918.24114844</v>
       </c>
       <c r="D51" t="n">
-        <v>5923046.40444792</v>
+        <v>5925626.75662767</v>
       </c>
       <c r="E51" t="n">
-        <v>2920818.01974628</v>
+        <v>2922090.78615444</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>6324295.12249529</v>
+        <v>6325832.5514612</v>
       </c>
       <c r="B52" t="n">
-        <v>1929766.92738698</v>
+        <v>1930231.20740547</v>
       </c>
       <c r="C52" t="n">
-        <v>3074128.06890756</v>
+        <v>3074881.62219445</v>
       </c>
       <c r="D52" t="n">
-        <v>5124465.51224934</v>
+        <v>5125755.37273855</v>
       </c>
       <c r="E52" t="n">
-        <v>2633700.23176688</v>
+        <v>2634359.70224628</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>17600068.1867043</v>
+        <v>17609473.7371614</v>
       </c>
       <c r="B53" t="n">
-        <v>1620274.25102924</v>
+        <v>1621056.34924122</v>
       </c>
       <c r="C53" t="n">
-        <v>5320300.43306575</v>
+        <v>5323139.58650431</v>
       </c>
       <c r="D53" t="n">
-        <v>5078503.21443077</v>
+        <v>5081311.04501877</v>
       </c>
       <c r="E53" t="n">
-        <v>1154016.58071865</v>
+        <v>1154655.58735596</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>23104927.301169</v>
+        <v>23103789.6873513</v>
       </c>
       <c r="B54" t="n">
-        <v>8244526.01632921</v>
+        <v>8244122.35303316</v>
       </c>
       <c r="C54" t="n">
-        <v>6090738.02933237</v>
+        <v>6090439.23181617</v>
       </c>
       <c r="D54" t="n">
-        <v>8508004.37541159</v>
+        <v>8507572.74609119</v>
       </c>
       <c r="E54" t="n">
-        <v>4249070.2718959</v>
+        <v>4248857.78770198</v>
       </c>
     </row>
     <row r="55">
@@ -3434,19 +3468,36 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>8885790.26768812</v>
+        <v>8907299.85150081</v>
       </c>
       <c r="B60" t="n">
-        <v>6069513.70615829</v>
+        <v>6124288.46252217</v>
       </c>
       <c r="C60" t="n">
-        <v>7095614.64760402</v>
+        <v>7180288.52753023</v>
       </c>
       <c r="D60" t="n">
-        <v>7725547.00071825</v>
+        <v>7368239.36550753</v>
       </c>
       <c r="E60" t="n">
-        <v>10657141.5200941</v>
+        <v>10860143.5076591</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>13692831.6743887</v>
+      </c>
+      <c r="B61" t="n">
+        <v>4660506.52180956</v>
+      </c>
+      <c r="C61" t="n">
+        <v>6475044.84813046</v>
+      </c>
+      <c r="D61" t="n">
+        <v>18220031.5526836</v>
+      </c>
+      <c r="E61" t="n">
+        <v>7560060.48227917</v>
       </c>
     </row>
   </sheetData>
@@ -3456,12 +3507,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -4468,19 +4519,36 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>8461494.92707114</v>
+        <v>8479724.71799159</v>
       </c>
       <c r="B60" t="n">
-        <v>5776402.50584379</v>
+        <v>5826972.84508351</v>
       </c>
       <c r="C60" t="n">
-        <v>6785280.23768978</v>
+        <v>6863945.90190409</v>
       </c>
       <c r="D60" t="n">
-        <v>7322840.46632597</v>
+        <v>6982907.01191293</v>
       </c>
       <c r="E60" t="n">
-        <v>10100440.3009972</v>
+        <v>10292908.0575963</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>13091748.1292148</v>
+      </c>
+      <c r="B61" t="n">
+        <v>4456931.02609038</v>
+      </c>
+      <c r="C61" t="n">
+        <v>6215990.20357408</v>
+      </c>
+      <c r="D61" t="n">
+        <v>17320585.6169122</v>
+      </c>
+      <c r="E61" t="n">
+        <v>7186631.23940244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>